<commit_message>
Adds LCIs of biochar, enhanced weathering of rock and ocean liming.
</commit_message>
<xml_diff>
--- a/premise/data/additional_inventories/lci-coastal-enhanced-weathering.xlsx
+++ b/premise/data/additional_inventories/lci-coastal-enhanced-weathering.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/romain/GitHub/premise/premise/data/additional_inventories/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE7DE04C-31D3-F942-B9C8-30F71FAA9411}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9AD05F7-23CD-F346-A175-2011470F9FB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="760" windowWidth="28080" windowHeight="18680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="cew_02102023" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">cew_02102023!$A$1:$H$54</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">cew_02102023!$A$1:$H$52</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="71">
   <si>
     <t>Database</t>
   </si>
@@ -113,12 +113,6 @@
     <t>Transformation, from grassland, natural (non-use)</t>
   </si>
   <si>
-    <t>Transformation, to forest, unspecified</t>
-  </si>
-  <si>
-    <t>Transformation, to grassland, natural (non-use)</t>
-  </si>
-  <si>
     <t>Transformation, to mineral extraction site</t>
   </si>
   <si>
@@ -227,7 +221,35 @@
     <t>olivine, unprocessed</t>
   </si>
   <si>
-    <t xml:space="preserve">This dataset represents the supply of 1 kg of olivine. In the paper it is assumed that an area of 200,000m2 will be mined over 50 years, with an annual capacity of 500 kt, i.e., 0.5 m2 for land use and 0.01 m2 per year for land use change are ascribed per FU. An average topsoil thickness of 0.2 m, with a bulk density of 1.3 t m−3, is considered, suggesting that 1.04 kt of overburden is produced year-round. For overburden handling, a bulldozer and a hydraulic shovel is considered, with the energy input taken from US Department of Energy, corresponding to activities in a surface limestone mine, whereas 200 km was ascribed for overburden transportation, used for backfilling. The quarry infrastructure was assumed to be similar to that of a gravel/sand quarry, as described in Kellenberger et al.
+    <t>olivine comminution</t>
+  </si>
+  <si>
+    <t>This dataset represents the grinding of 1 kilogram of olivine to a size of 10 µm. The transportation of rocks to the crushing/grinding facility at a distance of 10 km. In the paper, they use mining truck data from the ELCD database with an off-road transport payload of 220 t expressed in mass units. Instead of the mining truck in this inventory, we chose the "dirtiest" transportation mode available from ecoinvent v3.9.1. The electricity consumption includes the electricity needed for the vibrating feeder, conveyor belt, vibrating screen and crushing the mineral to 10µm.
+Foteinis, S., Campbell, J. S., &amp; Renforth, P. (2023). Life Cycle Assessment of Coastal Enhanced Weathering for Carbon Dioxide Removal from Air. Environmental Science and Technology, 57(15), 6169–6178. https://doi.org/10.1021/acs.est.2c08633</t>
+  </si>
+  <si>
+    <t>olivine, ground</t>
+  </si>
+  <si>
+    <t>carbon dioxide, captured and stored by olivine spreading on coastline</t>
+  </si>
+  <si>
+    <t>This dataset represents the spreading of 1 kilogram of crushed olivine to the coastal area. The crushed olivine is loaded in trucks and transported for an average of 50 km to the coastline to be spread using a lime spreader. The authors assume olivine to be spread on the dry beach width using standard lime-spreading equipment. They provide a unit in tonnes. In ecoinvent, though, the lime spreader is expressed in hectares. Therefore  we use a solid manure hydraulic spreader as a proxy technology expressed in kilograms, which has the very same technosphere and biosphere flows as the lime spreader. Source: Foteinis, S., Campbell, J. S., &amp; Renforth, P. (2023). Life Cycle Assessment of Coastal Enhanced Weathering for Carbon Dioxide Removal from Air. Environmental Science and Technology, 57(15), 6169–6178. https://doi.org/10.1021/acs.est.2c08633</t>
+  </si>
+  <si>
+    <t>Carbon dioxide, in air</t>
+  </si>
+  <si>
+    <t>olivine, spread on coastal area</t>
+  </si>
+  <si>
+    <t>natural resource::in air</t>
+  </si>
+  <si>
+    <t>Olivine</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This dataset represents the supply of 1 kg of olivine. In the paper it is assumed that an area of 200,000m2 will be mined over 50 years, with an annual capacity of 500 kt, i.e., 0.5 m2 for land use and 0.01 m2 per year for land use change are ascribed per FU. An average topsoil thickness of 0.2 m, with a bulk density of 1.3 t m−3, is considered, suggesting that 1.04 kt of overburden is produced year-round. For overburden handling, a bulldozer and a hydraulic shovel is considered, with the energy input taken from US Department of Energy, corresponding to activities in a surface limestone mine, whereas 200 km was ascribed for overburden transportation, used for backfilling. The quarry infrastructure was assumed to be similar to that of a gravel/sand quarry, as described in Kellenberger et al. Note that in the original publication, restauration is assumed after 50 years, and the land is transformed back into forest land. This asusmption is NOT made here.
 Source: Foteinis, S., Campbell, J. S., &amp; Renforth, P. (2023). Life Cycle Assessment of Coastal Enhanced Weathering for Carbon Dioxide Removal from Air. Environmental Science and Technology, 57(15), 6169–6178. https://doi.org/10.1021/acs.est.2c08633
 ****Additional comments****
 Diesel, represents the diesel amount used for bulldozer and hydraulic shovel for overburden handling, for drilling, the diesel used for trucks, graders and lighting for mining operations and  the energy input for loading. For the machinery used in quarrying (drill, service trucks, bulk trucks, and graders), Ecoinvent’s data for diesel burned in agricultural machinery, i.e., for running a tractor with a trailer, was used as a proxy.
@@ -236,34 +258,6 @@
 Lubricating oil used for drilling and loading. For rock drilling, the lubricating oil consumption is considered as described in Rosado et al.
 For water pumping, a mean energy of 0.45 kWh per m3 was ascribed for (borehole) water pumping (diesel-powered).
 </t>
-  </si>
-  <si>
-    <t>olivine comminution</t>
-  </si>
-  <si>
-    <t>This dataset represents the grinding of 1 kilogram of olivine to a size of 10 µm. The transportation of rocks to the crushing/grinding facility at a distance of 10 km. In the paper, they use mining truck data from the ELCD database with an off-road transport payload of 220 t expressed in mass units. Instead of the mining truck in this inventory, we chose the "dirtiest" transportation mode available from ecoinvent v3.9.1. The electricity consumption includes the electricity needed for the vibrating feeder, conveyor belt, vibrating screen and crushing the mineral to 10µm.
-Foteinis, S., Campbell, J. S., &amp; Renforth, P. (2023). Life Cycle Assessment of Coastal Enhanced Weathering for Carbon Dioxide Removal from Air. Environmental Science and Technology, 57(15), 6169–6178. https://doi.org/10.1021/acs.est.2c08633</t>
-  </si>
-  <si>
-    <t>olivine, ground</t>
-  </si>
-  <si>
-    <t>carbon dioxide, captured and stored by olivine spreading on coastline</t>
-  </si>
-  <si>
-    <t>This dataset represents the spreading of 1 kilogram of crushed olivine to the coastal area. The crushed olivine is loaded in trucks and transported for an average of 50 km to the coastline to be spread using a lime spreader. The authors assume olivine to be spread on the dry beach width using standard lime-spreading equipment. They provide a unit in tonnes. In ecoinvent, though, the lime spreader is expressed in hectares. Therefore  we use a solid manure hydraulic spreader as a proxy technology expressed in kilograms, which has the very same technosphere and biosphere flows as the lime spreader. Source: Foteinis, S., Campbell, J. S., &amp; Renforth, P. (2023). Life Cycle Assessment of Coastal Enhanced Weathering for Carbon Dioxide Removal from Air. Environmental Science and Technology, 57(15), 6169–6178. https://doi.org/10.1021/acs.est.2c08633</t>
-  </si>
-  <si>
-    <t>Carbon dioxide, in air</t>
-  </si>
-  <si>
-    <t>olivine, spread on coastal area</t>
-  </si>
-  <si>
-    <t>natural resource::in air</t>
-  </si>
-  <si>
-    <t>Olivine</t>
   </si>
 </sst>
 </file>
@@ -315,10 +309,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -623,10 +618,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H55"/>
+  <dimension ref="A1:H53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -647,15 +642,15 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
-        <v>63</v>
+      <c r="B4" s="3" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
@@ -671,7 +666,7 @@
         <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
@@ -723,7 +718,7 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B11">
         <v>1</v>
@@ -738,90 +733,90 @@
         <v>10</v>
       </c>
       <c r="G11" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H11" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B12">
         <v>1.3946771199999999E-2</v>
       </c>
       <c r="C12" t="s">
+        <v>31</v>
+      </c>
+      <c r="D12" t="s">
+        <v>32</v>
+      </c>
+      <c r="E12" t="s">
         <v>33</v>
       </c>
-      <c r="D12" t="s">
+      <c r="G12" t="s">
         <v>34</v>
       </c>
-      <c r="E12" t="s">
-        <v>35</v>
-      </c>
-      <c r="G12" t="s">
-        <v>36</v>
-      </c>
       <c r="H12" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B13">
         <v>3.9999999999999998E-11</v>
       </c>
       <c r="C13" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D13" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E13" t="s">
         <v>9</v>
       </c>
       <c r="G13" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="H13" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B14">
         <v>1.448E-4</v>
       </c>
       <c r="C14" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D14" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E14" t="s">
         <v>10</v>
       </c>
       <c r="G14" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="H14" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B15">
         <v>1.7519999999999999E-6</v>
       </c>
       <c r="C15" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D15" t="s">
         <v>5</v>
@@ -830,61 +825,61 @@
         <v>10</v>
       </c>
       <c r="G15" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="H15" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B16">
         <v>8.2399999999999997E-4</v>
       </c>
       <c r="C16" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D16" t="s">
         <v>5</v>
       </c>
       <c r="E16" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="G16" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="H16" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B17">
         <v>4.0484000000000001E-5</v>
       </c>
       <c r="C17" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D17" t="s">
         <v>5</v>
       </c>
       <c r="E17" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="G17" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="H17" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B18">
         <v>1</v>
@@ -967,7 +962,7 @@
         <v>25</v>
       </c>
       <c r="B22">
-        <v>2.0000000000000001E-4</v>
+        <v>4.0000000000000002E-4</v>
       </c>
       <c r="C22" t="s">
         <v>16</v>
@@ -987,488 +982,448 @@
         <v>26</v>
       </c>
       <c r="B23">
-        <v>2.0000000000000001E-4</v>
+        <v>7.1296000000000003E-5</v>
       </c>
       <c r="C23" t="s">
         <v>16</v>
       </c>
       <c r="E23" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="F23" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="G23" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
-        <v>27</v>
-      </c>
-      <c r="B24">
-        <v>4.0000000000000002E-4</v>
-      </c>
-      <c r="C24" t="s">
-        <v>16</v>
-      </c>
-      <c r="E24" t="s">
-        <v>23</v>
-      </c>
-      <c r="F24" t="s">
-        <v>21</v>
-      </c>
-      <c r="G24" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
-        <v>28</v>
-      </c>
-      <c r="B25">
-        <v>7.1296000000000003E-5</v>
-      </c>
-      <c r="C25" t="s">
-        <v>16</v>
-      </c>
-      <c r="E25" t="s">
-        <v>29</v>
-      </c>
-      <c r="F25" t="s">
-        <v>30</v>
-      </c>
-      <c r="G25" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="A27" s="1" t="s">
+    <row r="25" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A25" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B27" s="1" t="s">
-        <v>64</v>
+      <c r="B25" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>3</v>
+      </c>
+      <c r="B26" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>4</v>
+      </c>
+      <c r="B27" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B28" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B29" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
+        <v>9</v>
+      </c>
+      <c r="B30" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A31" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F32" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G32" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H32" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B30" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
-        <v>7</v>
-      </c>
-      <c r="B31" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
-        <v>9</v>
-      </c>
-      <c r="B32" t="s">
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>61</v>
+      </c>
+      <c r="B33">
+        <v>1</v>
+      </c>
+      <c r="C33" t="s">
+        <v>1</v>
+      </c>
+      <c r="D33" t="s">
+        <v>5</v>
+      </c>
+      <c r="E33" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="33" spans="1:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="A33" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B34" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C34" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D34" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E34" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F34" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="G34" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="H34" s="2" t="s">
-        <v>6</v>
+      <c r="G33" t="s">
+        <v>29</v>
+      </c>
+      <c r="H33" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>59</v>
+      </c>
+      <c r="B34">
+        <v>1</v>
+      </c>
+      <c r="C34" t="s">
+        <v>1</v>
+      </c>
+      <c r="D34" t="s">
+        <v>5</v>
+      </c>
+      <c r="E34" t="s">
+        <v>10</v>
+      </c>
+      <c r="G34" t="s">
+        <v>34</v>
+      </c>
+      <c r="H34" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>64</v>
+        <v>48</v>
       </c>
       <c r="B35">
-        <v>1</v>
+        <v>0.01</v>
       </c>
       <c r="C35" t="s">
-        <v>1</v>
+        <v>31</v>
       </c>
       <c r="D35" t="s">
-        <v>5</v>
+        <v>36</v>
       </c>
       <c r="E35" t="s">
-        <v>10</v>
+        <v>43</v>
       </c>
       <c r="G35" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="H35" t="s">
-        <v>66</v>
+        <v>49</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="B36">
-        <v>1</v>
+        <v>7.4455999999999994E-2</v>
       </c>
       <c r="C36" t="s">
-        <v>1</v>
+        <v>31</v>
       </c>
       <c r="D36" t="s">
         <v>5</v>
       </c>
       <c r="E36" t="s">
-        <v>10</v>
+        <v>46</v>
       </c>
       <c r="G36" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="H36" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>50</v>
+        <v>26</v>
       </c>
       <c r="B37">
-        <v>0.01</v>
+        <v>3.256E-4</v>
       </c>
       <c r="C37" t="s">
-        <v>33</v>
-      </c>
-      <c r="D37" t="s">
-        <v>38</v>
+        <v>16</v>
       </c>
       <c r="E37" t="s">
-        <v>45</v>
+        <v>27</v>
+      </c>
+      <c r="F37" t="s">
+        <v>28</v>
       </c>
       <c r="G37" t="s">
-        <v>36</v>
-      </c>
-      <c r="H37" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A38" t="s">
-        <v>52</v>
-      </c>
-      <c r="B38">
-        <v>7.4455999999999994E-2</v>
-      </c>
-      <c r="C38" t="s">
-        <v>33</v>
-      </c>
-      <c r="D38" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A39" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>3</v>
+      </c>
+      <c r="B40" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>4</v>
+      </c>
+      <c r="B41" t="s">
         <v>5</v>
-      </c>
-      <c r="E38" t="s">
-        <v>48</v>
-      </c>
-      <c r="G38" t="s">
-        <v>36</v>
-      </c>
-      <c r="H38" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A39" t="s">
-        <v>28</v>
-      </c>
-      <c r="B39">
-        <v>3.256E-4</v>
-      </c>
-      <c r="C39" t="s">
-        <v>16</v>
-      </c>
-      <c r="E39" t="s">
-        <v>29</v>
-      </c>
-      <c r="F39" t="s">
-        <v>30</v>
-      </c>
-      <c r="G39" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="A41" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B41" s="1" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B42" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B43" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
+        <v>9</v>
+      </c>
+      <c r="B44" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A45" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A46" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D46" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E46" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F46" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G46" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H46" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B44" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A45" t="s">
-        <v>7</v>
-      </c>
-      <c r="B45" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A46" t="s">
-        <v>9</v>
-      </c>
-      <c r="B46" t="s">
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>64</v>
+      </c>
+      <c r="B47">
+        <v>1</v>
+      </c>
+      <c r="C47" t="s">
+        <v>1</v>
+      </c>
+      <c r="D47" t="s">
+        <v>5</v>
+      </c>
+      <c r="E47" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="47" spans="1:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="A47" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B48" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C48" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D48" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E48" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F48" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="G48" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="H48" s="2" t="s">
-        <v>6</v>
+      <c r="G47" t="s">
+        <v>29</v>
+      </c>
+      <c r="H47" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>61</v>
+      </c>
+      <c r="B48">
+        <v>1.25</v>
+      </c>
+      <c r="C48" t="s">
+        <v>1</v>
+      </c>
+      <c r="D48" t="s">
+        <v>5</v>
+      </c>
+      <c r="E48" t="s">
+        <v>10</v>
+      </c>
+      <c r="G48" t="s">
+        <v>34</v>
+      </c>
+      <c r="H48" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>67</v>
+        <v>54</v>
       </c>
       <c r="B49">
-        <v>1</v>
+        <v>7.1639999999999994E-3</v>
       </c>
       <c r="C49" t="s">
-        <v>1</v>
+        <v>31</v>
       </c>
       <c r="D49" t="s">
-        <v>5</v>
+        <v>32</v>
       </c>
       <c r="E49" t="s">
-        <v>10</v>
+        <v>33</v>
       </c>
       <c r="G49" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="H49" t="s">
-        <v>70</v>
+        <v>30</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="B50">
         <v>1.25</v>
       </c>
       <c r="C50" t="s">
-        <v>1</v>
+        <v>31</v>
       </c>
       <c r="D50" t="s">
-        <v>5</v>
+        <v>32</v>
       </c>
       <c r="E50" t="s">
         <v>10</v>
       </c>
       <c r="G50" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="H50" t="s">
-        <v>66</v>
+        <v>56</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B51">
-        <v>7.1639999999999994E-3</v>
+        <v>6.25E-2</v>
       </c>
       <c r="C51" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D51" t="s">
+        <v>5</v>
+      </c>
+      <c r="E51" t="s">
+        <v>43</v>
+      </c>
+      <c r="G51" t="s">
         <v>34</v>
       </c>
-      <c r="E51" t="s">
-        <v>35</v>
-      </c>
-      <c r="G51" t="s">
-        <v>36</v>
-      </c>
       <c r="H51" t="s">
-        <v>32</v>
+        <v>58</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="B52">
-        <v>1.25</v>
+        <v>3.2899999999999995E-3</v>
       </c>
       <c r="C52" t="s">
-        <v>33</v>
-      </c>
-      <c r="D52" t="s">
-        <v>34</v>
+        <v>16</v>
       </c>
       <c r="E52" t="s">
         <v>10</v>
       </c>
+      <c r="F52" t="s">
+        <v>53</v>
+      </c>
       <c r="G52" t="s">
-        <v>36</v>
-      </c>
-      <c r="H52" t="s">
-        <v>58</v>
+        <v>18</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>59</v>
+        <v>66</v>
       </c>
       <c r="B53">
-        <v>6.25E-2</v>
+        <v>1</v>
       </c>
       <c r="C53" t="s">
-        <v>33</v>
-      </c>
-      <c r="D53" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="E53" t="s">
-        <v>45</v>
+        <v>10</v>
+      </c>
+      <c r="F53" t="s">
+        <v>68</v>
       </c>
       <c r="G53" t="s">
-        <v>36</v>
-      </c>
-      <c r="H53" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A54" t="s">
-        <v>54</v>
-      </c>
-      <c r="B54">
-        <v>3.2899999999999995E-3</v>
-      </c>
-      <c r="C54" t="s">
-        <v>16</v>
-      </c>
-      <c r="E54" t="s">
-        <v>10</v>
-      </c>
-      <c r="F54" t="s">
-        <v>55</v>
-      </c>
-      <c r="G54" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A55" t="s">
-        <v>69</v>
-      </c>
-      <c r="B55">
-        <v>1</v>
-      </c>
-      <c r="C55" t="s">
-        <v>16</v>
-      </c>
-      <c r="E55" t="s">
-        <v>10</v>
-      </c>
-      <c r="F55" t="s">
-        <v>71</v>
-      </c>
-      <c r="G55" t="s">
-        <v>18</v>
-      </c>
-    </row>
   </sheetData>
-  <autoFilter ref="A1:H54" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:H52" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>